<commit_message>
adding in 1-4 stuff
</commit_message>
<xml_diff>
--- a/handouts/chapter_1_4_handout.xlsx
+++ b/handouts/chapter_1_4_handout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RussellStuff\Time series personal work\timeseries\handouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5434BC-7C42-4021-BACA-6F65D8634CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D83CA26-CEE7-4228-9F01-109894F175A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB73943A-C465-40BE-817C-B9991112161C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{CB73943A-C465-40BE-817C-B9991112161C}"/>
   </bookViews>
   <sheets>
     <sheet name="Workbook" sheetId="2" r:id="rId1"/>
@@ -384,7 +384,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,8 +403,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -566,6 +572,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -581,7 +602,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -655,6 +675,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4284,37 +4305,37 @@
   <dimension ref="A1:N113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.90625" customWidth="1"/>
+    <col min="14" max="14" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:4" ht="45.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="27"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" s="17"/>
+      <c r="D2" s="26"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -4328,7 +4349,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -4342,7 +4363,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -4356,7 +4377,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -4370,7 +4391,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -4384,7 +4405,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -4398,7 +4419,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -4408,9 +4429,9 @@
       <c r="C9" s="1">
         <v>3351.5833333333335</v>
       </c>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="39"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -4420,9 +4441,9 @@
       <c r="C10" s="1">
         <v>3350</v>
       </c>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -4432,9 +4453,9 @@
       <c r="C11" s="1">
         <v>3343.2083333333335</v>
       </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="39"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -4444,9 +4465,9 @@
       <c r="C12" s="1">
         <v>3326.2083333333335</v>
       </c>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -4456,9 +4477,9 @@
       <c r="C13" s="1">
         <v>3316.5416666666665</v>
       </c>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" s="39"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -4468,9 +4489,9 @@
       <c r="C14" s="1">
         <v>3318.5833333333335</v>
       </c>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="39"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -4480,9 +4501,9 @@
       <c r="C15" s="1">
         <v>3312.0833333333335</v>
       </c>
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15" s="39"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -4492,9 +4513,9 @@
       <c r="C16" s="1">
         <v>3308.0416666666665</v>
       </c>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -4504,11 +4525,11 @@
       <c r="C17" s="1">
         <v>3311.7083333333335</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>-296.70833333333348</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
@@ -4518,11 +4539,11 @@
       <c r="C18" s="1">
         <v>3313.1666666666665</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>-334.16666666666652</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -4532,11 +4553,11 @@
       <c r="C19" s="1">
         <v>3307.75</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>135.25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
@@ -4546,11 +4567,11 @@
       <c r="C20" s="1">
         <v>3292.4166666666665</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>221.58333333333348</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
@@ -4560,11 +4581,11 @@
       <c r="C21" s="1">
         <v>3281.0833333333335</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>270.91666666666652</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
@@ -4574,11 +4595,11 @@
       <c r="C22" s="1">
         <v>3270.2083333333335</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <v>219.79166666666652</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
@@ -4588,11 +4609,11 @@
       <c r="C23" s="1">
         <v>3259.4583333333335</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <v>319.54166666666652</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -4602,11 +4623,11 @@
       <c r="C24" s="1">
         <v>3261.1666666666665</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="8">
         <v>395.83333333333348</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
@@ -4616,11 +4637,11 @@
       <c r="C25" s="1">
         <v>3264.25</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="8">
         <v>-14.25</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
@@ -4630,11 +4651,11 @@
       <c r="C26" s="1">
         <v>3260.4583333333335</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="8">
         <v>-79.458333333333485</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -4644,11 +4665,11 @@
       <c r="C27" s="1">
         <v>3256.7083333333335</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="8">
         <v>-308.70833333333348</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -4658,11 +4679,11 @@
       <c r="C28" s="1">
         <v>3262.125</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="8">
         <v>-727.125</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
@@ -4672,11 +4693,11 @@
       <c r="C29" s="1">
         <v>3267.0833333333335</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="8">
         <v>-311.08333333333348</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -4686,11 +4707,11 @@
       <c r="C30" s="1">
         <v>3259.2916666666665</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="8">
         <v>-180.29166666666652</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
@@ -4700,11 +4721,11 @@
       <c r="C31" s="1">
         <v>3254</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="8">
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
@@ -4714,11 +4735,11 @@
       <c r="C32" s="1">
         <v>3256.9583333333335</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="8">
         <v>192.04166666666652</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
@@ -4728,11 +4749,11 @@
       <c r="C33" s="1">
         <v>3256.7083333333335</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="8">
         <v>270.29166666666652</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
@@ -4742,11 +4763,11 @@
       <c r="C34" s="1">
         <v>3269</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="8">
         <v>376</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>36</v>
       </c>
@@ -4756,11 +4777,11 @@
       <c r="C35" s="1">
         <v>3279.0833333333335</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="8">
         <v>263.91666666666652</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
@@ -4770,11 +4791,11 @@
       <c r="C36" s="1">
         <v>3252.8333333333335</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="8">
         <v>253.16666666666652</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
@@ -4784,11 +4805,11 @@
       <c r="C37" s="1">
         <v>3228.0416666666665</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="8">
         <v>45.958333333333485</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
@@ -4798,11 +4819,11 @@
       <c r="C38" s="1">
         <v>3248.2083333333335</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="8">
         <v>-20.208333333333485</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
@@ -4812,11 +4833,11 @@
       <c r="C39" s="1">
         <v>3294.2916666666665</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="8">
         <v>-399.29166666666652</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>41</v>
       </c>
@@ -4826,11 +4847,11 @@
       <c r="C40" s="1">
         <v>3340.3333333333335</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="8">
         <v>-457.33333333333348</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>42</v>
       </c>
@@ -4840,11 +4861,11 @@
       <c r="C41" s="1">
         <v>3384.6666666666665</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="8">
         <v>-534.66666666666652</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>43</v>
       </c>
@@ -4854,11 +4875,11 @@
       <c r="C42" s="1">
         <v>3433.5416666666665</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="8">
         <v>-878.54166666666652</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
@@ -4868,11 +4889,11 @@
       <c r="C43" s="1">
         <v>3481.2916666666665</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="8">
         <v>-135.29166666666652</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>45</v>
       </c>
@@ -4882,11 +4903,11 @@
       <c r="C44" s="1">
         <v>3514.8333333333335</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="8">
         <v>489.16666666666652</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>46</v>
       </c>
@@ -4896,11 +4917,11 @@
       <c r="C45" s="1">
         <v>3549.875</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="8">
         <v>528.125</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
@@ -4910,11 +4931,11 @@
       <c r="C46" s="1">
         <v>3567.7083333333335</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="8">
         <v>631.29166666666652</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>48</v>
       </c>
@@ -4924,11 +4945,11 @@
       <c r="C47" s="1">
         <v>3590.6666666666665</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="8">
         <v>462.33333333333348</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>49</v>
       </c>
@@ -4938,11 +4959,11 @@
       <c r="C48" s="1">
         <v>3672.125</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="8">
         <v>496.875</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>50</v>
       </c>
@@ -4952,11 +4973,11 @@
       <c r="C49" s="1">
         <v>3758.1666666666665</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="8">
         <v>-1.1666666666665151</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>51</v>
       </c>
@@ -4966,11 +4987,11 @@
       <c r="C50" s="1">
         <v>3793.7916666666665</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="8">
         <v>-243.79166666666652</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>52</v>
       </c>
@@ -4980,11 +5001,11 @@
       <c r="C51" s="1">
         <v>3804.8333333333335</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="8">
         <v>-390.83333333333348</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>53</v>
       </c>
@@ -4994,11 +5015,11 @@
       <c r="C52" s="1">
         <v>3816.625</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52" s="8">
         <v>-1024.625</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>54</v>
       </c>
@@ -5008,11 +5029,11 @@
       <c r="C53" s="1">
         <v>3830.9583333333335</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="8">
         <v>-338.95833333333348</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>55</v>
       </c>
@@ -5022,11 +5043,11 @@
       <c r="C54" s="1">
         <v>3853.2916666666665</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="8">
         <v>14.708333333333485</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>56</v>
       </c>
@@ -5036,11 +5057,11 @@
       <c r="C55" s="1">
         <v>3875.5</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="8">
         <v>222.5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>57</v>
       </c>
@@ -5050,11 +5071,11 @@
       <c r="C56" s="1">
         <v>3899.8333333333335</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D56" s="8">
         <v>207.16666666666652</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>58</v>
       </c>
@@ -5068,7 +5089,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>59</v>
       </c>
@@ -5082,7 +5103,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>60</v>
       </c>
@@ -5096,7 +5117,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>61</v>
       </c>
@@ -5110,7 +5131,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>62</v>
       </c>
@@ -5124,82 +5145,82 @@
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="14">
+      <c r="B62" s="13">
         <v>3914</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C62" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="35" t="s">
+    <row r="65" spans="1:14" ht="34.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="36"/>
-      <c r="I65" s="36"/>
-      <c r="J65" s="36"/>
-      <c r="K65" s="36"/>
-      <c r="L65" s="36"/>
-      <c r="M65" s="36"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="35"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="35"/>
+      <c r="H65" s="35"/>
+      <c r="I65" s="35"/>
+      <c r="J65" s="35"/>
+      <c r="K65" s="35"/>
+      <c r="L65" s="35"/>
+      <c r="M65" s="35"/>
       <c r="N65" s="3"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A66" s="28" t="s">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A66" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="23" t="s">
+      <c r="B66" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="23" t="s">
+      <c r="C66" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D66" s="23" t="s">
+      <c r="D66" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="E66" s="23" t="s">
+      <c r="E66" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F66" s="23" t="s">
+      <c r="F66" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="G66" s="23" t="s">
+      <c r="G66" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="H66" s="23" t="s">
+      <c r="H66" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="I66" s="23" t="s">
+      <c r="I66" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="J66" s="23" t="s">
+      <c r="J66" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="K66" s="23" t="s">
+      <c r="K66" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="L66" s="23" t="s">
+      <c r="L66" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="M66" s="24" t="s">
+      <c r="M66" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="N66" s="10"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A67" s="29">
+      <c r="N66" s="9"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A67" s="28">
         <v>2017</v>
       </c>
       <c r="B67" t="s">
@@ -5220,20 +5241,20 @@
       <c r="G67" t="s">
         <v>79</v>
       </c>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="9"/>
-      <c r="N67" s="11"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A68" s="29">
+      <c r="H67" s="39"/>
+      <c r="I67" s="39"/>
+      <c r="J67" s="39"/>
+      <c r="K67" s="39"/>
+      <c r="L67" s="39"/>
+      <c r="M67" s="39"/>
+      <c r="N67" s="10"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A68" s="28">
         <v>2018</v>
       </c>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
       <c r="D68" s="1">
         <v>-296.70833333333348</v>
       </c>
@@ -5261,13 +5282,13 @@
       <c r="L68" s="1">
         <v>-14.25</v>
       </c>
-      <c r="M68" s="9">
+      <c r="M68" s="8">
         <v>-79.458333333333485</v>
       </c>
-      <c r="N68" s="11"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A69" s="29">
+      <c r="N68" s="10"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A69" s="28">
         <v>2019</v>
       </c>
       <c r="B69" s="1">
@@ -5303,13 +5324,13 @@
       <c r="L69" s="1">
         <v>45.958333333333485</v>
       </c>
-      <c r="M69" s="9">
+      <c r="M69" s="8">
         <v>-20.208333333333485</v>
       </c>
-      <c r="N69" s="11"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A70" s="29">
+      <c r="N69" s="10"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A70" s="28">
         <v>2020</v>
       </c>
       <c r="B70" s="1">
@@ -5345,15 +5366,15 @@
       <c r="L70" s="1">
         <v>-1.1666666666665151</v>
       </c>
-      <c r="M70" s="9">
+      <c r="M70" s="8">
         <v>-243.79166666666652</v>
       </c>
-      <c r="N70" s="30" t="s">
+      <c r="N70" s="29" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A71" s="29">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A71" s="28">
         <v>2021</v>
       </c>
       <c r="B71" s="1">
@@ -5392,10 +5413,10 @@
       <c r="M71" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="N71" s="31"/>
-    </row>
-    <row r="72" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="25" t="s">
+      <c r="N71" s="30"/>
+    </row>
+    <row r="72" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="24" t="s">
         <v>77</v>
       </c>
       <c r="B72" s="1">
@@ -5428,59 +5449,59 @@
       <c r="K72" s="1">
         <v>362.16666666666663</v>
       </c>
-      <c r="L72" s="1"/>
-      <c r="M72" s="9"/>
-      <c r="N72" s="12">
+      <c r="L72" s="39"/>
+      <c r="M72" s="39"/>
+      <c r="N72" s="11">
         <v>-5.0060763888889142</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="26"/>
+    <row r="73" spans="1:14" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="25"/>
       <c r="B73" s="7">
         <v>-345.22309027777783</v>
       </c>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="7"/>
-      <c r="I73" s="7"/>
-      <c r="J73" s="7"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="7"/>
-      <c r="M73" s="8"/>
-      <c r="N73" s="13"/>
-    </row>
-    <row r="76" spans="1:14" ht="43.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="32" t="s">
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="39"/>
+      <c r="H73" s="39"/>
+      <c r="I73" s="39"/>
+      <c r="J73" s="39"/>
+      <c r="K73" s="39"/>
+      <c r="L73" s="39"/>
+      <c r="M73" s="39"/>
+      <c r="N73" s="12"/>
+    </row>
+    <row r="76" spans="1:14" ht="43.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="B76" s="33"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="34"/>
-    </row>
-    <row r="77" spans="1:14" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="19" t="s">
+      <c r="B76" s="32"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="32"/>
+      <c r="G76" s="33"/>
+    </row>
+    <row r="77" spans="1:14" ht="37.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="21" t="s">
+      <c r="C77" s="20"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G77" s="22" t="s">
+      <c r="G77" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>4</v>
       </c>
@@ -5493,13 +5514,13 @@
       <c r="D78" t="s">
         <v>79</v>
       </c>
-      <c r="E78" s="1"/>
+      <c r="E78" s="39"/>
       <c r="F78" t="s">
         <v>79</v>
       </c>
-      <c r="G78" s="9"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G78" s="39"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>5</v>
       </c>
@@ -5512,13 +5533,13 @@
       <c r="D79" t="s">
         <v>79</v>
       </c>
-      <c r="E79" s="1"/>
+      <c r="E79" s="39"/>
       <c r="F79" t="s">
         <v>79</v>
       </c>
-      <c r="G79" s="9"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G79" s="39"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>6</v>
       </c>
@@ -5531,13 +5552,13 @@
       <c r="D80" t="s">
         <v>79</v>
       </c>
-      <c r="E80" s="1"/>
+      <c r="E80" s="39"/>
       <c r="F80" t="s">
         <v>79</v>
       </c>
-      <c r="G80" s="9"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G80" s="39"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>7</v>
       </c>
@@ -5550,13 +5571,13 @@
       <c r="D81" t="s">
         <v>79</v>
       </c>
-      <c r="E81" s="1"/>
+      <c r="E81" s="39"/>
       <c r="F81" t="s">
         <v>79</v>
       </c>
-      <c r="G81" s="9"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G81" s="39"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>8</v>
       </c>
@@ -5569,13 +5590,13 @@
       <c r="D82" t="s">
         <v>79</v>
       </c>
-      <c r="E82" s="1"/>
+      <c r="E82" s="39"/>
       <c r="F82" t="s">
         <v>79</v>
       </c>
-      <c r="G82" s="9"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G82" s="39"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>9</v>
       </c>
@@ -5588,13 +5609,13 @@
       <c r="D83" t="s">
         <v>79</v>
       </c>
-      <c r="E83" s="1"/>
+      <c r="E83" s="39"/>
       <c r="F83" t="s">
         <v>79</v>
       </c>
-      <c r="G83" s="9"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G83" s="39"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>10</v>
       </c>
@@ -5607,11 +5628,11 @@
       <c r="D84" s="1">
         <v>378.41666666666652</v>
       </c>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="9"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E84" s="39"/>
+      <c r="F84" s="39"/>
+      <c r="G84" s="39"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>11</v>
       </c>
@@ -5624,11 +5645,11 @@
       <c r="D85" s="1">
         <v>59</v>
       </c>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="9"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E85" s="39"/>
+      <c r="F85" s="39"/>
+      <c r="G85" s="39"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>12</v>
       </c>
@@ -5641,11 +5662,11 @@
       <c r="D86" s="1">
         <v>228.79166666666652</v>
       </c>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="9"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E86" s="39"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="39"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>13</v>
       </c>
@@ -5658,11 +5679,11 @@
       <c r="D87" s="1">
         <v>302.79166666666652</v>
       </c>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="9"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E87" s="39"/>
+      <c r="F87" s="39"/>
+      <c r="G87" s="39"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>14</v>
       </c>
@@ -5675,11 +5696,11 @@
       <c r="D88" s="1">
         <v>91.458333333333485</v>
       </c>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="9"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E88" s="39"/>
+      <c r="F88" s="39"/>
+      <c r="G88" s="39"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>15</v>
       </c>
@@ -5692,11 +5713,11 @@
       <c r="D89" s="1">
         <v>72.416666666666515</v>
       </c>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="9"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E89" s="39"/>
+      <c r="F89" s="39"/>
+      <c r="G89" s="39"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>16</v>
       </c>
@@ -5709,11 +5730,11 @@
       <c r="D90" s="1">
         <v>-302.08333333333348</v>
       </c>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="9"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E90" s="39"/>
+      <c r="F90" s="39"/>
+      <c r="G90" s="39"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>17</v>
       </c>
@@ -5726,11 +5747,11 @@
       <c r="D91" s="1">
         <v>-574.04166666666652</v>
       </c>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="9"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E91" s="39"/>
+      <c r="F91" s="39"/>
+      <c r="G91" s="39"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>18</v>
       </c>
@@ -5743,11 +5764,11 @@
       <c r="D92" s="1">
         <v>-296.70833333333348</v>
       </c>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="9"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E92" s="39"/>
+      <c r="F92" s="39"/>
+      <c r="G92" s="39"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
         <v>19</v>
       </c>
@@ -5760,11 +5781,11 @@
       <c r="D93" s="1">
         <v>-334.16666666666652</v>
       </c>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="9"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E93" s="39"/>
+      <c r="F93" s="39"/>
+      <c r="G93" s="39"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>20</v>
       </c>
@@ -5783,11 +5804,12 @@
       <c r="F94" s="1">
         <v>33.879340277777715</v>
       </c>
-      <c r="G94" s="9">
+      <c r="G94" s="8">
         <v>3341.6293402777778</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>21</v>
       </c>
@@ -5806,11 +5828,11 @@
       <c r="F95" s="1">
         <v>-60.912326388888687</v>
       </c>
-      <c r="G95" s="9">
+      <c r="G95" s="8">
         <v>3231.5043402777778</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>22</v>
       </c>
@@ -5829,11 +5851,11 @@
       <c r="F96" s="1">
         <v>-96.026909722222285</v>
       </c>
-      <c r="G96" s="9">
+      <c r="G96" s="8">
         <v>3185.0564236111113</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
         <v>23</v>
       </c>
@@ -5852,11 +5874,11 @@
       <c r="F97" s="1">
         <v>-106.73524305555566</v>
       </c>
-      <c r="G97" s="9">
+      <c r="G97" s="8">
         <v>3163.4730902777778</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>24</v>
       </c>
@@ -5875,11 +5897,11 @@
       <c r="F98" s="1">
         <v>-4.1102430555556566</v>
       </c>
-      <c r="G98" s="9">
+      <c r="G98" s="8">
         <v>3255.3480902777778</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>25</v>
       </c>
@@ -5898,11 +5920,11 @@
       <c r="F99" s="1">
         <v>28.660590277777942</v>
       </c>
-      <c r="G99" s="9">
+      <c r="G99" s="8">
         <v>3289.8272569444443</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>26</v>
       </c>
@@ -5921,11 +5943,11 @@
       <c r="F100" s="1">
         <v>-49.756076388889028</v>
       </c>
-      <c r="G100" s="9">
+      <c r="G100" s="8">
         <v>3214.4939236111109</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>27</v>
       </c>
@@ -5944,20 +5966,20 @@
       <c r="F101" s="1">
         <v>-16.703993055555657</v>
       </c>
-      <c r="G101" s="9">
+      <c r="G101" s="8">
         <v>3243.7543402777778</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="6"/>
-      <c r="B102" s="14"/>
-      <c r="C102" s="14"/>
-      <c r="D102" s="14"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14"/>
-      <c r="G102" s="15"/>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B102" s="13"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="14"/>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
@@ -5965,7 +5987,7 @@
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -5979,7 +6001,7 @@
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -5993,7 +6015,7 @@
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -6007,7 +6029,7 @@
       <c r="L110" s="1"/>
       <c r="M110" s="1"/>
     </row>
-    <row r="111" spans="1:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
@@ -6015,7 +6037,7 @@
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A112" s="2"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -6030,7 +6052,7 @@
       <c r="L112" s="1"/>
       <c r="M112" s="1"/>
     </row>
-    <row r="113" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -6060,20 +6082,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ca1cba85-b018-40b2-9d9a-243cd5b6fae5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ca1cba85-b018-40b2-9d9a-243cd5b6fae5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6272,6 +6294,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C96E0334-A0AA-41B5-AE21-CAD1C9D10746}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5E1B631-90B0-4D19-A35E-F8DC8BE167A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -6284,14 +6314,6 @@
     <ds:schemaRef ds:uri="f1fb8133-dfcb-4ab3-83e1-bcafde3f766a"/>
     <ds:schemaRef ds:uri="ca1cba85-b018-40b2-9d9a-243cd5b6fae5"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C96E0334-A0AA-41B5-AE21-CAD1C9D10746}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>